<commit_message>
Added separate all race files
</commit_message>
<xml_diff>
--- a/dps_dashboard/data/2021/school_stats_data/race.xlsx
+++ b/dps_dashboard/data/2021/school_stats_data/race.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/scholar/Desktop/Visualizing DPS/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\poona\Desktop\College Doc Dump\Data+\New Repo\visualizing_DPS\dps_dashboard\data\2021\school_stats_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EAAB31E4-EFAF-D947-88CE-8F1AFF7A6946}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBF78073-6286-40E7-B9A0-D506CEBDFEDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1160" yWindow="500" windowWidth="27640" windowHeight="15640" xr2:uid="{8A77730F-63B3-7A4A-B171-15DB83AB20AC}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8A77730F-63B3-7A4A-B171-15DB83AB20AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -471,17 +471,17 @@
   <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="24.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.69921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.69921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -492,7 +492,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -503,7 +503,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -514,7 +514,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -525,7 +525,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -536,7 +536,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>14</v>
       </c>
@@ -547,7 +547,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>14</v>
       </c>
@@ -558,7 +558,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>3</v>
       </c>
@@ -569,7 +569,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>3</v>
       </c>
@@ -580,7 +580,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>4</v>
       </c>
@@ -591,7 +591,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>4</v>
       </c>
@@ -602,7 +602,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>5</v>
       </c>
@@ -613,7 +613,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>5</v>
       </c>
@@ -624,7 +624,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>6</v>
       </c>
@@ -636,7 +636,7 @@
       </c>
       <c r="H14" s="1"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>6</v>
       </c>
@@ -648,7 +648,7 @@
       </c>
       <c r="H15" s="1"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>7</v>
       </c>
@@ -660,7 +660,7 @@
       </c>
       <c r="H16" s="1"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>7</v>
       </c>
@@ -672,7 +672,7 @@
       </c>
       <c r="H17" s="1"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>8</v>
       </c>
@@ -685,7 +685,7 @@
       <c r="D18" s="4"/>
       <c r="H18" s="1"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>8</v>
       </c>
@@ -698,7 +698,7 @@
       <c r="D19" s="4"/>
       <c r="H19" s="1"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>9</v>
       </c>
@@ -711,7 +711,7 @@
       <c r="D20" s="4"/>
       <c r="H20" s="1"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>9</v>
       </c>
@@ -724,28 +724,28 @@
       <c r="D21" s="5"/>
       <c r="H21" s="2"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C22" s="3"/>
       <c r="D22" s="4"/>
       <c r="H22" s="1"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C23" s="3"/>
       <c r="D23" s="4"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C24" s="3"/>
       <c r="D24" s="4"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C25" s="3"/>
       <c r="D25" s="4"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C26" s="3"/>
       <c r="D26" s="4"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C27" s="3"/>
       <c r="D27" s="5"/>
     </row>

</xml_diff>